<commit_message>
plain soda leerzeichen entfernt
</commit_message>
<xml_diff>
--- a/helper_skripts/menu_converter/menu-2024.12.14.xlsx
+++ b/helper_skripts/menu_converter/menu-2024.12.14.xlsx
@@ -457,7 +457,7 @@
     <t>Gazoz Çeşitleri</t>
   </si>
   <si>
-    <t xml:space="preserve">Plain Soda </t>
+    <t>Plain Soda</t>
   </si>
   <si>
     <t>Sade Soda</t>
@@ -3249,7 +3249,7 @@
         <v>10</v>
       </c>
       <c r="B97" s="7"/>
-      <c r="C97" s="7" t="s">
+      <c r="C97" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D97" s="17"/>

</xml_diff>